<commit_message>
cuongdq push by sh
</commit_message>
<xml_diff>
--- a/db/excel/admin-user-baoduong-tram.xlsx
+++ b/db/excel/admin-user-baoduong-tram.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CCC85EF-E292-431C-9544-9D0F644342F8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D119EB0A-CA6C-44DC-966C-0615D4070E93}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="103">
   <si>
     <t>type</t>
   </si>
@@ -98,12 +98,6 @@
   </si>
   <si>
     <t>Trạng thái bấm chuột?? Default true</t>
-  </si>
-  <si>
-    <t>default true</t>
-  </si>
-  <si>
-    <t>BOOLEAN</t>
   </si>
   <si>
     <t>next</t>
@@ -772,280 +766,280 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="274">
-    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="91" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="93" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="103" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="107" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="109" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="111" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="113" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="117" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="119" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="121" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="123" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="125" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="127" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="129" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="131" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="133" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="135" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="137" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="139" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="141" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="143" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="145" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="147" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="149" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="151" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="153" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="155" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="157" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="159" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="161" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="163" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="165" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="167" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="169" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="171" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="173" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="175" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="177" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="179" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="181" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="183" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="185" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="187" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="189" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="191" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="193" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="195" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="197" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="199" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="201" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="203" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="205" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="207" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="209" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="211" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="213" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="215" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="217" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="219" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="221" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="223" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="225" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="227" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="229" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="231" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="233" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="235" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="237" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="239" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="241" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="243" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="245" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="247" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="249" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="251" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="253" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="255" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="257" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="259" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="261" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="263" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="265" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="267" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="269" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="271" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="273" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="32" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="34" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="36" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="38" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="40" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="52" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="54" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="62" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="64" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="66" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="68" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="70" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="72" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="74" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="76" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="78" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="80" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="82" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="84" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="86" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="88" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="90" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="92" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="94" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="96" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="98" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="100" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="102" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="104" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="106" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="108" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="110" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="112" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="114" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="116" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="118" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="120" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="122" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="124" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="126" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="128" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="130" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="132" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="134" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="136" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="138" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="140" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="142" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="144" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="146" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="148" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="150" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="152" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="154" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="156" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="158" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="160" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="162" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="164" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="166" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="168" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="170" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="172" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="174" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="176" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="178" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="180" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="182" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="184" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="186" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="188" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="190" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="192" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="194" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="196" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="198" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="200" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="202" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="204" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="206" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="208" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="210" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="212" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="214" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="216" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="218" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="220" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="222" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="224" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="226" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="228" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="230" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="232" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="234" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="236" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="238" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="240" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="242" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="244" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="246" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="248" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="250" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="252" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="254" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="256" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="258" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="260" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="262" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="264" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="266" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="268" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="270" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="272" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000011010000}"/>
+    <cellStyle name="Siêu kết nối" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="6" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="8" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="10" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="12" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="14" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="16" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="18" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="20" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="22" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="24" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="26" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="28" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="30" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="32" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="34" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="36" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="38" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="40" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="42" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="48" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="50" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="52" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="54" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="56" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="58" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="60" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="62" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="64" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="66" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="68" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="70" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="72" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="74" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="76" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="78" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="80" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="82" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="84" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="86" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="88" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="90" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="92" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="94" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="96" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="98" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="100" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="102" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="104" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="106" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="108" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="110" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="112" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="114" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="116" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="118" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="120" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="122" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="124" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="126" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="128" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="130" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="132" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="134" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="136" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="138" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="140" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="142" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="144" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="146" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="148" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="150" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="152" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="154" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="156" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="158" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="160" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="162" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="164" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="166" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="168" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="170" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="172" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="174" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="176" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="178" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="180" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="182" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="184" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="186" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="188" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="190" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="192" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="194" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="196" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="198" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="200" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="202" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="204" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="206" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="208" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="210" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="212" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="214" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="216" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="218" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="220" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="222" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="224" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="226" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="228" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="230" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="232" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="234" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="236" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="238" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="240" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="242" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="244" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="246" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="248" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="250" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="252" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="254" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="256" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="258" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="260" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="262" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="264" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="266" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="268" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="270" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối" xfId="272" builtinId="8" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="41" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="75" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="81" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="87" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="89" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="91" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="93" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="107" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="109" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="111" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="113" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="115" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="117" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="119" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="121" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="123" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="125" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="127" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="129" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="131" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="133" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="135" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="137" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="139" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="141" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="143" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="145" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="147" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="149" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="151" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="153" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="155" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="157" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="159" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="161" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="163" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="165" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="167" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="169" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="171" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="173" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="175" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="177" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="179" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="181" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="183" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="185" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="187" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="189" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="191" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="193" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="195" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="197" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="199" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="201" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="203" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="205" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="207" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="209" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="211" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="213" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="215" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="217" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="219" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="221" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="223" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="225" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="227" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="229" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="231" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="233" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="235" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="237" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="239" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="241" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="243" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="245" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="247" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="249" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="251" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="253" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="255" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="257" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="259" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="261" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="263" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="265" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="267" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="269" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="271" builtinId="9" hidden="1"/>
+    <cellStyle name="Siêu kết nối đã Bấm vào" xfId="273" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -1350,7 +1344,7 @@
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -1391,7 +1385,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>8</v>
@@ -1438,7 +1432,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>9</v>
@@ -1453,7 +1447,7 @@
         <v>13</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>8</v>
@@ -1486,10 +1480,10 @@
         <v>23</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75">
@@ -1497,10 +1491,10 @@
         <v>16</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>9</v>
@@ -1512,10 +1506,10 @@
         <v>16</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>9</v>
@@ -1527,10 +1521,10 @@
         <v>16</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>9</v>
@@ -1545,7 +1539,7 @@
         <v>0</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>9</v>
@@ -1557,10 +1551,10 @@
         <v>16</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>36</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>8</v>
@@ -1572,10 +1566,10 @@
         <v>16</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>35</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>8</v>
@@ -1601,13 +1595,13 @@
     </row>
     <row r="16" spans="1:6" s="5" customFormat="1" ht="15.75">
       <c r="A16" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>8</v>
@@ -1618,13 +1612,13 @@
     </row>
     <row r="17" spans="1:5" s="5" customFormat="1" ht="15.75">
       <c r="A17" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>9</v>
@@ -1632,13 +1626,13 @@
     </row>
     <row r="18" spans="1:5" s="5" customFormat="1" ht="15.75">
       <c r="A18" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>9</v>
@@ -1647,13 +1641,13 @@
     </row>
     <row r="19" spans="1:5" s="5" customFormat="1" ht="15.75">
       <c r="A19" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>8</v>
@@ -1662,13 +1656,13 @@
     </row>
     <row r="20" spans="1:5" s="5" customFormat="1" ht="15.75">
       <c r="A20" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>8</v>
@@ -1677,7 +1671,7 @@
     </row>
     <row r="21" spans="1:5" s="5" customFormat="1" ht="15.75">
       <c r="A21" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>1</v>
@@ -1689,7 +1683,7 @@
         <v>8</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:5" s="8" customFormat="1">
@@ -1697,10 +1691,10 @@
         <v>15</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D22" s="8" t="s">
         <v>9</v>
@@ -1711,10 +1705,10 @@
         <v>15</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D23" s="8" t="s">
         <v>9</v>
@@ -1725,10 +1719,10 @@
         <v>15</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D24" s="8" t="s">
         <v>9</v>
@@ -1739,10 +1733,10 @@
         <v>15</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D25" s="8" t="s">
         <v>8</v>
@@ -1753,10 +1747,10 @@
         <v>15</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D26" s="8" t="s">
         <v>8</v>
@@ -1770,13 +1764,13 @@
         <v>1</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D27" s="8" t="s">
         <v>8</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1795,7 +1789,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
@@ -1836,22 +1830,22 @@
         <v>22</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I1" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" s="13" t="s">
         <v>27</v>
-      </c>
-      <c r="J1" s="13" t="s">
-        <v>29</v>
       </c>
       <c r="K1" s="13" t="s">
         <v>0</v>
       </c>
       <c r="L1" s="13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="M1" s="13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="N1" s="13" t="s">
         <v>1</v>
@@ -1863,26 +1857,26 @@
       </c>
       <c r="B2" s="15"/>
       <c r="C2" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2" s="15">
+        <v>1</v>
+      </c>
+      <c r="F2" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="D2" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="E2" s="15">
-        <v>1</v>
-      </c>
-      <c r="F2" s="17" t="s">
+      <c r="G2" s="15">
+        <v>1</v>
+      </c>
+      <c r="H2" s="18" t="s">
         <v>55</v>
-      </c>
-      <c r="G2" s="15">
-        <v>1</v>
-      </c>
-      <c r="H2" s="18" t="s">
-        <v>57</v>
       </c>
       <c r="I2" s="15"/>
       <c r="J2" s="17" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="K2" s="15"/>
       <c r="L2" s="15"/>
@@ -1897,26 +1891,26 @@
       </c>
       <c r="B3" s="15"/>
       <c r="C3" s="15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E3" s="15">
         <v>2</v>
       </c>
       <c r="F3" s="17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G3" s="15">
         <v>1</v>
       </c>
       <c r="H3" s="18" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I3" s="15"/>
       <c r="J3" s="17" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K3" s="15"/>
       <c r="L3" s="15"/>
@@ -1931,26 +1925,26 @@
       </c>
       <c r="B4" s="15"/>
       <c r="C4" s="15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E4" s="15">
         <v>3</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G4" s="15">
         <v>1</v>
       </c>
       <c r="H4" s="18" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="I4" s="15"/>
       <c r="J4" s="17" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="K4" s="15"/>
       <c r="L4" s="15"/>
@@ -1965,26 +1959,26 @@
       </c>
       <c r="B5" s="15"/>
       <c r="C5" s="15" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E5" s="15">
         <v>4</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G5" s="15">
         <v>1</v>
       </c>
       <c r="H5" s="18" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="I5" s="15"/>
       <c r="J5" s="17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="K5" s="15"/>
       <c r="L5" s="15"/>
@@ -1999,26 +1993,26 @@
       </c>
       <c r="B6" s="15"/>
       <c r="C6" s="15" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E6" s="15">
         <v>5</v>
       </c>
       <c r="F6" s="17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G6" s="15">
         <v>1</v>
       </c>
       <c r="H6" s="19" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="I6" s="15"/>
       <c r="J6" s="17" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="K6" s="15"/>
       <c r="L6" s="15"/>
@@ -2033,26 +2027,26 @@
       </c>
       <c r="B7" s="15"/>
       <c r="C7" s="15" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E7" s="15">
         <v>6</v>
       </c>
       <c r="F7" s="17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G7" s="15">
         <v>1</v>
       </c>
       <c r="H7" s="19" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I7" s="15"/>
       <c r="J7" s="17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K7" s="15"/>
       <c r="L7" s="15"/>
@@ -2067,26 +2061,26 @@
       </c>
       <c r="B8" s="15"/>
       <c r="C8" s="15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E8" s="15">
         <v>7</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G8" s="15">
         <v>1</v>
       </c>
       <c r="H8" s="18" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="I8" s="15"/>
       <c r="J8" s="17" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="K8" s="15"/>
       <c r="L8" s="15"/>
@@ -2101,26 +2095,26 @@
       </c>
       <c r="B9" s="15"/>
       <c r="C9" s="15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E9" s="15">
         <v>8</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G9" s="15">
         <v>1</v>
       </c>
       <c r="H9" s="18" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I9" s="15"/>
       <c r="J9" s="17" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="K9" s="15"/>
       <c r="L9" s="15"/>
@@ -2144,9 +2138,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
@@ -2163,16 +2155,16 @@
         <v>2</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>1</v>
@@ -2183,10 +2175,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F2" s="10">
         <v>1</v>
@@ -2197,10 +2189,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -2208,13 +2200,13 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -2222,13 +2214,13 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -2236,13 +2228,13 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -2250,13 +2242,13 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F7">
         <v>1</v>
@@ -2264,13 +2256,13 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -2278,13 +2270,13 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F9">
         <v>1</v>
@@ -2316,19 +2308,19 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>48</v>
-      </c>
       <c r="D1" s="8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F1" s="8" t="s">
         <v>1</v>
@@ -2339,7 +2331,7 @@
         <v>702418821</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F2">
         <v>1</v>

</xml_diff>